<commit_message>
recommender server connection to recommender algorithm
</commit_message>
<xml_diff>
--- a/Data/dataframe1.xlsx
+++ b/Data/dataframe1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w2980\Desktop\graduation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1F76E3-97D5-4927-8E74-B52AB9388F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563F23E7-A2C6-4C76-BA91-2DCADBC28AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13710" yWindow="1455" windowWidth="15390" windowHeight="12090" xr2:uid="{C4C6211A-2526-4C5B-B6A6-1AFBBEB271E2}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="14400" windowHeight="15600" xr2:uid="{C4C6211A-2526-4C5B-B6A6-1AFBBEB271E2}"/>
   </bookViews>
   <sheets>
     <sheet name="woman" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="64">
   <si>
     <t>p_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -212,6 +212,36 @@
   </si>
   <si>
     <t>맨투맨</t>
+  </si>
+  <si>
+    <t>soom._.inc</t>
+  </si>
+  <si>
+    <t>컨버스</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>조끼</t>
+  </si>
+  <si>
+    <t>블레이저</t>
+  </si>
+  <si>
+    <t>1,5,7</t>
+  </si>
+  <si>
+    <t>바람막이</t>
+  </si>
+  <si>
+    <t>5,7</t>
+  </si>
+  <si>
+    <t>니트집업</t>
+  </si>
+  <si>
+    <t>치마바지</t>
   </si>
 </sst>
 </file>
@@ -685,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EA69EE-38A5-477D-AF99-E56B73E9C5A8}">
-  <dimension ref="B1:L103"/>
+  <dimension ref="B1:L158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="L151" sqref="L151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1465,21 +1495,6 @@
       <c r="C37" t="s">
         <v>11</v>
       </c>
-      <c r="D37">
-        <v>7</v>
-      </c>
-      <c r="F37" t="s">
-        <v>32</v>
-      </c>
-      <c r="H37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" t="s">
-        <v>31</v>
-      </c>
-      <c r="J37">
-        <v>22</v>
-      </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38">
@@ -2884,7 +2899,1329 @@
       <c r="L102" s="6"/>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>54</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="F103" t="s">
+        <v>29</v>
+      </c>
+      <c r="H103" t="s">
+        <v>13</v>
+      </c>
+      <c r="I103" t="s">
+        <v>55</v>
+      </c>
+      <c r="J103">
+        <v>28</v>
+      </c>
       <c r="L103" s="6"/>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>54</v>
+      </c>
+      <c r="D104">
+        <v>7</v>
+      </c>
+      <c r="F104" t="s">
+        <v>29</v>
+      </c>
+      <c r="G104" t="s">
+        <v>56</v>
+      </c>
+      <c r="H104" t="s">
+        <v>13</v>
+      </c>
+      <c r="I104" t="s">
+        <v>27</v>
+      </c>
+      <c r="J104">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>54</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="F105" t="s">
+        <v>29</v>
+      </c>
+      <c r="H105" t="s">
+        <v>13</v>
+      </c>
+      <c r="I105" t="s">
+        <v>27</v>
+      </c>
+      <c r="J105">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>4</v>
+      </c>
+      <c r="C106" t="s">
+        <v>54</v>
+      </c>
+      <c r="D106" t="s">
+        <v>36</v>
+      </c>
+      <c r="F106" t="s">
+        <v>12</v>
+      </c>
+      <c r="H106" t="s">
+        <v>13</v>
+      </c>
+      <c r="I106" t="s">
+        <v>27</v>
+      </c>
+      <c r="J106">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>54</v>
+      </c>
+      <c r="D107">
+        <v>4</v>
+      </c>
+      <c r="F107" t="s">
+        <v>20</v>
+      </c>
+      <c r="H107" t="s">
+        <v>13</v>
+      </c>
+      <c r="I107" t="s">
+        <v>24</v>
+      </c>
+      <c r="J107">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>6</v>
+      </c>
+      <c r="C108" t="s">
+        <v>54</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="F108" t="s">
+        <v>53</v>
+      </c>
+      <c r="H108" t="s">
+        <v>37</v>
+      </c>
+      <c r="I108" t="s">
+        <v>31</v>
+      </c>
+      <c r="J108">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s">
+        <v>54</v>
+      </c>
+      <c r="D109" t="s">
+        <v>36</v>
+      </c>
+      <c r="F109" t="s">
+        <v>32</v>
+      </c>
+      <c r="H109" t="s">
+        <v>13</v>
+      </c>
+      <c r="I109" t="s">
+        <v>31</v>
+      </c>
+      <c r="J109">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>8</v>
+      </c>
+      <c r="C110" t="s">
+        <v>54</v>
+      </c>
+      <c r="D110" t="s">
+        <v>36</v>
+      </c>
+      <c r="F110" t="s">
+        <v>53</v>
+      </c>
+      <c r="H110" t="s">
+        <v>13</v>
+      </c>
+      <c r="I110" t="s">
+        <v>31</v>
+      </c>
+      <c r="J110">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>9</v>
+      </c>
+      <c r="C111" t="s">
+        <v>54</v>
+      </c>
+      <c r="D111" t="s">
+        <v>36</v>
+      </c>
+      <c r="F111" t="s">
+        <v>57</v>
+      </c>
+      <c r="H111" t="s">
+        <v>13</v>
+      </c>
+      <c r="I111" t="s">
+        <v>55</v>
+      </c>
+      <c r="J111">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>10</v>
+      </c>
+      <c r="C112" t="s">
+        <v>54</v>
+      </c>
+      <c r="D112" t="s">
+        <v>51</v>
+      </c>
+      <c r="E112" t="s">
+        <v>58</v>
+      </c>
+      <c r="F112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H112" t="s">
+        <v>13</v>
+      </c>
+      <c r="I112" t="s">
+        <v>24</v>
+      </c>
+      <c r="J112">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>11</v>
+      </c>
+      <c r="C113" t="s">
+        <v>54</v>
+      </c>
+      <c r="D113" t="s">
+        <v>51</v>
+      </c>
+      <c r="E113" t="s">
+        <v>50</v>
+      </c>
+      <c r="H113" t="s">
+        <v>37</v>
+      </c>
+      <c r="I113" t="s">
+        <v>55</v>
+      </c>
+      <c r="J113">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>12</v>
+      </c>
+      <c r="C114" t="s">
+        <v>54</v>
+      </c>
+      <c r="D114" t="s">
+        <v>59</v>
+      </c>
+      <c r="F114" t="s">
+        <v>32</v>
+      </c>
+      <c r="H114" t="s">
+        <v>13</v>
+      </c>
+      <c r="I114" t="s">
+        <v>31</v>
+      </c>
+      <c r="J114">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>13</v>
+      </c>
+      <c r="C115" t="s">
+        <v>54</v>
+      </c>
+      <c r="D115" t="s">
+        <v>33</v>
+      </c>
+      <c r="F115" t="s">
+        <v>12</v>
+      </c>
+      <c r="H115" t="s">
+        <v>13</v>
+      </c>
+      <c r="I115" t="s">
+        <v>24</v>
+      </c>
+      <c r="J115">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>14</v>
+      </c>
+      <c r="C116" t="s">
+        <v>54</v>
+      </c>
+      <c r="D116">
+        <v>7</v>
+      </c>
+      <c r="F116" t="s">
+        <v>32</v>
+      </c>
+      <c r="G116" t="s">
+        <v>12</v>
+      </c>
+      <c r="H116" t="s">
+        <v>13</v>
+      </c>
+      <c r="I116" t="s">
+        <v>31</v>
+      </c>
+      <c r="J116">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>15</v>
+      </c>
+      <c r="C117" t="s">
+        <v>54</v>
+      </c>
+      <c r="D117" t="s">
+        <v>59</v>
+      </c>
+      <c r="F117" t="s">
+        <v>17</v>
+      </c>
+      <c r="H117" t="s">
+        <v>13</v>
+      </c>
+      <c r="I117" t="s">
+        <v>31</v>
+      </c>
+      <c r="J117">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>16</v>
+      </c>
+      <c r="C118" t="s">
+        <v>54</v>
+      </c>
+      <c r="D118">
+        <v>5</v>
+      </c>
+      <c r="E118" t="s">
+        <v>49</v>
+      </c>
+      <c r="H118" t="s">
+        <v>13</v>
+      </c>
+      <c r="I118" t="s">
+        <v>31</v>
+      </c>
+      <c r="J118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>17</v>
+      </c>
+      <c r="C119" t="s">
+        <v>54</v>
+      </c>
+      <c r="D119" t="s">
+        <v>36</v>
+      </c>
+      <c r="F119" t="s">
+        <v>32</v>
+      </c>
+      <c r="H119" t="s">
+        <v>13</v>
+      </c>
+      <c r="I119" t="s">
+        <v>55</v>
+      </c>
+      <c r="J119">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>18</v>
+      </c>
+      <c r="C120" t="s">
+        <v>54</v>
+      </c>
+      <c r="D120" t="s">
+        <v>36</v>
+      </c>
+      <c r="F120" t="s">
+        <v>32</v>
+      </c>
+      <c r="H120" t="s">
+        <v>13</v>
+      </c>
+      <c r="I120" t="s">
+        <v>31</v>
+      </c>
+      <c r="J120">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>19</v>
+      </c>
+      <c r="C121" t="s">
+        <v>54</v>
+      </c>
+      <c r="D121" t="s">
+        <v>59</v>
+      </c>
+      <c r="F121" t="s">
+        <v>17</v>
+      </c>
+      <c r="H121" t="s">
+        <v>13</v>
+      </c>
+      <c r="I121" t="s">
+        <v>55</v>
+      </c>
+      <c r="J121">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="122" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>20</v>
+      </c>
+      <c r="C122" t="s">
+        <v>54</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="F122" t="s">
+        <v>17</v>
+      </c>
+      <c r="H122" t="s">
+        <v>13</v>
+      </c>
+      <c r="I122" t="s">
+        <v>24</v>
+      </c>
+      <c r="J122">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="123" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>21</v>
+      </c>
+      <c r="C123" t="s">
+        <v>54</v>
+      </c>
+      <c r="D123">
+        <v>4</v>
+      </c>
+      <c r="F123" t="s">
+        <v>32</v>
+      </c>
+      <c r="H123" t="s">
+        <v>13</v>
+      </c>
+      <c r="I123" t="s">
+        <v>24</v>
+      </c>
+      <c r="J123">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="124" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>22</v>
+      </c>
+      <c r="C124" t="s">
+        <v>54</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="F124" t="s">
+        <v>17</v>
+      </c>
+      <c r="H124" t="s">
+        <v>13</v>
+      </c>
+      <c r="I124" t="s">
+        <v>31</v>
+      </c>
+      <c r="J124">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B125">
+        <v>23</v>
+      </c>
+      <c r="C125" t="s">
+        <v>54</v>
+      </c>
+      <c r="D125" t="s">
+        <v>36</v>
+      </c>
+      <c r="F125" t="s">
+        <v>32</v>
+      </c>
+      <c r="H125" t="s">
+        <v>13</v>
+      </c>
+      <c r="I125" t="s">
+        <v>55</v>
+      </c>
+      <c r="J125">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>24</v>
+      </c>
+      <c r="C126" t="s">
+        <v>54</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="F126" t="s">
+        <v>17</v>
+      </c>
+      <c r="H126" t="s">
+        <v>13</v>
+      </c>
+      <c r="I126" t="s">
+        <v>31</v>
+      </c>
+      <c r="J126">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="127" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>25</v>
+      </c>
+      <c r="C127" t="s">
+        <v>54</v>
+      </c>
+      <c r="D127" t="s">
+        <v>33</v>
+      </c>
+      <c r="E127" t="s">
+        <v>58</v>
+      </c>
+      <c r="F127" t="s">
+        <v>17</v>
+      </c>
+      <c r="H127" t="s">
+        <v>13</v>
+      </c>
+      <c r="I127" t="s">
+        <v>55</v>
+      </c>
+      <c r="J127">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>26</v>
+      </c>
+      <c r="C128" t="s">
+        <v>54</v>
+      </c>
+      <c r="D128" t="s">
+        <v>33</v>
+      </c>
+      <c r="E128" t="s">
+        <v>23</v>
+      </c>
+      <c r="F128" t="s">
+        <v>17</v>
+      </c>
+      <c r="H128" t="s">
+        <v>13</v>
+      </c>
+      <c r="I128" t="s">
+        <v>31</v>
+      </c>
+      <c r="J128">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>27</v>
+      </c>
+      <c r="C129" t="s">
+        <v>54</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="F129" t="s">
+        <v>17</v>
+      </c>
+      <c r="G129" t="s">
+        <v>17</v>
+      </c>
+      <c r="H129" t="s">
+        <v>13</v>
+      </c>
+      <c r="I129" t="s">
+        <v>31</v>
+      </c>
+      <c r="J129">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="130" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>28</v>
+      </c>
+      <c r="C130" t="s">
+        <v>54</v>
+      </c>
+      <c r="D130" t="s">
+        <v>33</v>
+      </c>
+      <c r="E130" t="s">
+        <v>60</v>
+      </c>
+      <c r="F130" t="s">
+        <v>29</v>
+      </c>
+      <c r="H130" t="s">
+        <v>13</v>
+      </c>
+      <c r="I130" t="s">
+        <v>31</v>
+      </c>
+      <c r="J130">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>29</v>
+      </c>
+      <c r="C131" t="s">
+        <v>54</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="F131" t="s">
+        <v>17</v>
+      </c>
+      <c r="H131" t="s">
+        <v>13</v>
+      </c>
+      <c r="I131" t="s">
+        <v>31</v>
+      </c>
+      <c r="J131">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="132" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>30</v>
+      </c>
+      <c r="C132" t="s">
+        <v>54</v>
+      </c>
+      <c r="D132" t="s">
+        <v>61</v>
+      </c>
+      <c r="E132" t="s">
+        <v>62</v>
+      </c>
+      <c r="F132" t="s">
+        <v>17</v>
+      </c>
+      <c r="H132" t="s">
+        <v>13</v>
+      </c>
+      <c r="I132" t="s">
+        <v>31</v>
+      </c>
+      <c r="J132">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="133" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>31</v>
+      </c>
+      <c r="C133" t="s">
+        <v>54</v>
+      </c>
+      <c r="D133" t="s">
+        <v>59</v>
+      </c>
+      <c r="F133" t="s">
+        <v>17</v>
+      </c>
+      <c r="G133" t="s">
+        <v>17</v>
+      </c>
+      <c r="H133" t="s">
+        <v>13</v>
+      </c>
+      <c r="I133" t="s">
+        <v>55</v>
+      </c>
+      <c r="J133">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="134" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>32</v>
+      </c>
+      <c r="C134" t="s">
+        <v>54</v>
+      </c>
+      <c r="D134">
+        <v>4</v>
+      </c>
+      <c r="F134" t="s">
+        <v>14</v>
+      </c>
+      <c r="I134" t="s">
+        <v>24</v>
+      </c>
+      <c r="J134">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="135" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>33</v>
+      </c>
+      <c r="C135" t="s">
+        <v>54</v>
+      </c>
+      <c r="D135" t="s">
+        <v>33</v>
+      </c>
+      <c r="F135" t="s">
+        <v>17</v>
+      </c>
+      <c r="H135" t="s">
+        <v>13</v>
+      </c>
+      <c r="I135" t="s">
+        <v>31</v>
+      </c>
+      <c r="J135">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="136" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>34</v>
+      </c>
+      <c r="C136" t="s">
+        <v>54</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="F136" t="s">
+        <v>20</v>
+      </c>
+      <c r="G136" t="s">
+        <v>29</v>
+      </c>
+      <c r="H136" t="s">
+        <v>13</v>
+      </c>
+      <c r="I136" t="s">
+        <v>55</v>
+      </c>
+      <c r="J136">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="137" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>35</v>
+      </c>
+      <c r="C137" t="s">
+        <v>54</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="F137" t="s">
+        <v>29</v>
+      </c>
+      <c r="H137" t="s">
+        <v>13</v>
+      </c>
+      <c r="I137" t="s">
+        <v>31</v>
+      </c>
+      <c r="J137">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="138" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>36</v>
+      </c>
+      <c r="C138" t="s">
+        <v>54</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="F138" t="s">
+        <v>17</v>
+      </c>
+      <c r="H138" t="s">
+        <v>13</v>
+      </c>
+      <c r="I138" t="s">
+        <v>31</v>
+      </c>
+      <c r="J138">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="139" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>37</v>
+      </c>
+      <c r="C139" t="s">
+        <v>54</v>
+      </c>
+      <c r="D139" t="s">
+        <v>33</v>
+      </c>
+      <c r="E139" t="s">
+        <v>60</v>
+      </c>
+      <c r="H139" t="s">
+        <v>13</v>
+      </c>
+      <c r="I139" t="s">
+        <v>31</v>
+      </c>
+      <c r="J139">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>38</v>
+      </c>
+      <c r="C140" t="s">
+        <v>54</v>
+      </c>
+      <c r="D140" t="s">
+        <v>33</v>
+      </c>
+      <c r="F140" t="s">
+        <v>17</v>
+      </c>
+      <c r="H140" t="s">
+        <v>13</v>
+      </c>
+      <c r="I140" t="s">
+        <v>27</v>
+      </c>
+      <c r="J140">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="141" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>39</v>
+      </c>
+      <c r="C141" t="s">
+        <v>54</v>
+      </c>
+      <c r="D141" t="s">
+        <v>33</v>
+      </c>
+      <c r="F141" t="s">
+        <v>17</v>
+      </c>
+      <c r="H141" t="s">
+        <v>13</v>
+      </c>
+      <c r="I141" t="s">
+        <v>31</v>
+      </c>
+      <c r="J141">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="142" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>40</v>
+      </c>
+      <c r="C142" t="s">
+        <v>54</v>
+      </c>
+      <c r="D142" t="s">
+        <v>33</v>
+      </c>
+      <c r="F142" t="s">
+        <v>17</v>
+      </c>
+      <c r="H142" t="s">
+        <v>13</v>
+      </c>
+      <c r="I142" t="s">
+        <v>31</v>
+      </c>
+      <c r="J142">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="143" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B143">
+        <v>41</v>
+      </c>
+      <c r="C143" t="s">
+        <v>54</v>
+      </c>
+      <c r="D143" t="s">
+        <v>33</v>
+      </c>
+      <c r="F143" t="s">
+        <v>29</v>
+      </c>
+      <c r="H143" t="s">
+        <v>13</v>
+      </c>
+      <c r="I143" t="s">
+        <v>31</v>
+      </c>
+      <c r="J143">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="144" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B144">
+        <v>42</v>
+      </c>
+      <c r="C144" t="s">
+        <v>54</v>
+      </c>
+      <c r="D144" t="s">
+        <v>33</v>
+      </c>
+      <c r="F144" t="s">
+        <v>29</v>
+      </c>
+      <c r="G144" t="s">
+        <v>17</v>
+      </c>
+      <c r="H144" t="s">
+        <v>13</v>
+      </c>
+      <c r="I144" t="s">
+        <v>31</v>
+      </c>
+      <c r="J144">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="145" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B145">
+        <v>43</v>
+      </c>
+      <c r="C145" t="s">
+        <v>54</v>
+      </c>
+      <c r="D145">
+        <v>4</v>
+      </c>
+      <c r="E145" t="s">
+        <v>58</v>
+      </c>
+      <c r="F145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H145" t="s">
+        <v>13</v>
+      </c>
+      <c r="I145" t="s">
+        <v>24</v>
+      </c>
+      <c r="J145">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B146">
+        <v>44</v>
+      </c>
+      <c r="C146" t="s">
+        <v>54</v>
+      </c>
+      <c r="D146" t="s">
+        <v>33</v>
+      </c>
+      <c r="F146" t="s">
+        <v>17</v>
+      </c>
+      <c r="H146" t="s">
+        <v>13</v>
+      </c>
+      <c r="I146" t="s">
+        <v>55</v>
+      </c>
+      <c r="J146">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="147" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B147">
+        <v>45</v>
+      </c>
+      <c r="C147" t="s">
+        <v>54</v>
+      </c>
+      <c r="D147" t="s">
+        <v>33</v>
+      </c>
+      <c r="F147" t="s">
+        <v>17</v>
+      </c>
+      <c r="H147" t="s">
+        <v>13</v>
+      </c>
+      <c r="I147" t="s">
+        <v>31</v>
+      </c>
+      <c r="J147">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="148" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B148">
+        <v>46</v>
+      </c>
+      <c r="C148" t="s">
+        <v>54</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148" t="s">
+        <v>62</v>
+      </c>
+      <c r="H148" t="s">
+        <v>13</v>
+      </c>
+      <c r="I148" t="s">
+        <v>31</v>
+      </c>
+      <c r="J148">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="149" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B149">
+        <v>47</v>
+      </c>
+      <c r="C149" t="s">
+        <v>54</v>
+      </c>
+      <c r="D149" t="s">
+        <v>33</v>
+      </c>
+      <c r="F149" t="s">
+        <v>17</v>
+      </c>
+      <c r="H149" t="s">
+        <v>13</v>
+      </c>
+      <c r="I149" t="s">
+        <v>31</v>
+      </c>
+      <c r="J149">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="150" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B150">
+        <v>48</v>
+      </c>
+      <c r="C150" t="s">
+        <v>54</v>
+      </c>
+      <c r="D150" t="s">
+        <v>33</v>
+      </c>
+      <c r="F150" t="s">
+        <v>29</v>
+      </c>
+      <c r="H150" t="s">
+        <v>13</v>
+      </c>
+      <c r="I150" t="s">
+        <v>55</v>
+      </c>
+      <c r="J150">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="151" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B151">
+        <v>49</v>
+      </c>
+      <c r="C151" t="s">
+        <v>54</v>
+      </c>
+      <c r="D151" t="s">
+        <v>33</v>
+      </c>
+      <c r="F151" t="s">
+        <v>20</v>
+      </c>
+      <c r="G151" t="s">
+        <v>29</v>
+      </c>
+      <c r="H151" t="s">
+        <v>13</v>
+      </c>
+      <c r="I151" t="s">
+        <v>55</v>
+      </c>
+      <c r="J151">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="152" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B152">
+        <v>50</v>
+      </c>
+      <c r="C152" t="s">
+        <v>54</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="F152" t="s">
+        <v>29</v>
+      </c>
+      <c r="H152" t="s">
+        <v>37</v>
+      </c>
+      <c r="I152" t="s">
+        <v>55</v>
+      </c>
+      <c r="J152">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="153" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B153">
+        <v>51</v>
+      </c>
+      <c r="C153" t="s">
+        <v>54</v>
+      </c>
+      <c r="D153">
+        <v>4</v>
+      </c>
+      <c r="F153" t="s">
+        <v>29</v>
+      </c>
+      <c r="H153" t="s">
+        <v>63</v>
+      </c>
+      <c r="I153" t="s">
+        <v>24</v>
+      </c>
+      <c r="J153">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="154" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B154">
+        <v>52</v>
+      </c>
+      <c r="C154" t="s">
+        <v>54</v>
+      </c>
+      <c r="D154" t="s">
+        <v>33</v>
+      </c>
+      <c r="F154" t="s">
+        <v>29</v>
+      </c>
+      <c r="H154" t="s">
+        <v>13</v>
+      </c>
+      <c r="I154" t="s">
+        <v>55</v>
+      </c>
+      <c r="J154">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="155" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B155">
+        <v>53</v>
+      </c>
+      <c r="C155" t="s">
+        <v>54</v>
+      </c>
+      <c r="D155" t="s">
+        <v>33</v>
+      </c>
+      <c r="F155" t="s">
+        <v>29</v>
+      </c>
+      <c r="H155" t="s">
+        <v>13</v>
+      </c>
+      <c r="I155" t="s">
+        <v>31</v>
+      </c>
+      <c r="J155">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="156" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B156">
+        <v>54</v>
+      </c>
+      <c r="C156" t="s">
+        <v>54</v>
+      </c>
+      <c r="D156" t="s">
+        <v>33</v>
+      </c>
+      <c r="F156" t="s">
+        <v>29</v>
+      </c>
+      <c r="H156" t="s">
+        <v>37</v>
+      </c>
+      <c r="I156" t="s">
+        <v>27</v>
+      </c>
+      <c r="J156">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="157" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B157">
+        <v>55</v>
+      </c>
+      <c r="C157" t="s">
+        <v>54</v>
+      </c>
+      <c r="D157" t="s">
+        <v>33</v>
+      </c>
+      <c r="F157" t="s">
+        <v>17</v>
+      </c>
+      <c r="H157" t="s">
+        <v>13</v>
+      </c>
+      <c r="I157" t="s">
+        <v>31</v>
+      </c>
+      <c r="J157">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="158" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B158">
+        <v>56</v>
+      </c>
+      <c r="C158" t="s">
+        <v>54</v>
+      </c>
+      <c r="D158">
+        <v>7</v>
+      </c>
+      <c r="F158" t="s">
+        <v>29</v>
+      </c>
+      <c r="H158" t="s">
+        <v>18</v>
+      </c>
+      <c r="I158" t="s">
+        <v>27</v>
+      </c>
+      <c r="J158">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>